<commit_message>
Memory deallocation bug fix
</commit_message>
<xml_diff>
--- a/doc/allocation.xlsx
+++ b/doc/allocation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\meka\CommanderX16Version\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{795A5A21-34C0-447B-87A2-79BEF4198879}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CF2F461-7DA0-409F-84B9-A2C9A59FA0A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="34620" windowHeight="14020" activeTab="1" xr2:uid="{02454ED2-5616-494F-84FC-2DE3FC8B32E3}"/>
+    <workbookView xWindow="430" yWindow="2080" windowWidth="18790" windowHeight="8130" xr2:uid="{02454ED2-5616-494F-84FC-2DE3FC8B32E3}"/>
   </bookViews>
   <sheets>
     <sheet name="Dynamic" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="42">
   <si>
     <t>Type</t>
   </si>
@@ -154,6 +154,15 @@
   </si>
   <si>
     <t>getNumTemp</t>
+  </si>
+  <si>
+    <t>Bank Segment</t>
+  </si>
+  <si>
+    <t>Segments Per Bank</t>
+  </si>
+  <si>
+    <t>Segment Calc</t>
   </si>
 </sst>
 </file>
@@ -197,11 +206,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -516,23 +524,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{355DE0EA-5B2C-4635-84EE-7D1B81ED29C7}">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.140625" customWidth="1"/>
-    <col min="5" max="5" width="9.42578125" customWidth="1"/>
+    <col min="1" max="1" width="16.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.1796875" customWidth="1"/>
+    <col min="5" max="5" width="9.453125" customWidth="1"/>
     <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -559,7 +567,7 @@
       </c>
       <c r="I1" s="1"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -586,7 +594,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -616,7 +624,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -646,7 +654,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -676,7 +684,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -706,7 +714,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>2</v>
       </c>
@@ -725,6 +733,32 @@
       <c r="F9">
         <f>SUM(F2:F6)</f>
         <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>40</v>
+      </c>
+      <c r="B15">
+        <f>C4/F4</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>41</v>
+      </c>
+      <c r="B16">
+        <f>(22-18) * B15 + B14</f>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -737,18 +771,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{382A0DF3-A6E2-4E63-819F-0B238C4B218B}">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" customWidth="1"/>
-    <col min="2" max="2" width="6.140625" customWidth="1"/>
-    <col min="3" max="4" width="11.42578125" customWidth="1"/>
+    <col min="1" max="1" width="19.81640625" customWidth="1"/>
+    <col min="2" max="2" width="6.1796875" customWidth="1"/>
+    <col min="3" max="4" width="11.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -766,7 +800,7 @@
       </c>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>35</v>
       </c>
@@ -783,7 +817,7 @@
         <v>7042</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>36</v>
       </c>
@@ -802,7 +836,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -821,7 +855,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>37</v>
       </c>
@@ -840,7 +874,7 @@
         <v>633</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>2</v>
       </c>
@@ -859,17 +893,17 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="A1:XFD1048576"/>
+      <selection activeCell="B5" sqref="B5:B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" customWidth="1"/>
-    <col min="2" max="2" width="6.140625" customWidth="1"/>
-    <col min="3" max="4" width="11.42578125" customWidth="1"/>
+    <col min="1" max="1" width="19.81640625" customWidth="1"/>
+    <col min="2" max="2" width="6.1796875" customWidth="1"/>
+    <col min="3" max="4" width="11.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -887,7 +921,7 @@
       </c>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>33</v>
       </c>
@@ -905,7 +939,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>34</v>
       </c>
@@ -921,11 +955,11 @@
         <v>400</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3:E9" si="1">C3*D3</f>
+        <f t="shared" ref="E3" si="1">C3*D3</f>
         <v>3600</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>2</v>
       </c>
@@ -948,14 +982,14 @@
       <selection activeCell="E9" sqref="A9:E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" customWidth="1"/>
-    <col min="2" max="2" width="6.140625" customWidth="1"/>
-    <col min="3" max="4" width="11.42578125" customWidth="1"/>
+    <col min="1" max="1" width="19.81640625" customWidth="1"/>
+    <col min="2" max="2" width="6.1796875" customWidth="1"/>
+    <col min="3" max="4" width="11.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -973,7 +1007,7 @@
       </c>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -991,12 +1025,12 @@
         <v>185</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>16</v>
       </c>
       <c r="B3">
-        <f>B2+ E2+1</f>
+        <f t="shared" ref="B3:B9" si="0">B2+ E2+1</f>
         <v>186</v>
       </c>
       <c r="C3">
@@ -1006,16 +1040,16 @@
         <v>255</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3:E6" si="0">C3*D3</f>
+        <f t="shared" ref="E3:E6" si="1">C3*D3</f>
         <v>1275</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>17</v>
       </c>
       <c r="B4">
-        <f>B3+ E3+1</f>
+        <f t="shared" si="0"/>
         <v>1462</v>
       </c>
       <c r="C4">
@@ -1025,16 +1059,16 @@
         <v>255</v>
       </c>
       <c r="E4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1275</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>18</v>
       </c>
       <c r="B5">
-        <f>B4+ E4+1</f>
+        <f t="shared" si="0"/>
         <v>2738</v>
       </c>
       <c r="C5">
@@ -1044,16 +1078,16 @@
         <v>255</v>
       </c>
       <c r="E5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1275</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>24</v>
       </c>
       <c r="B6">
-        <f>B5+ E5+1</f>
+        <f t="shared" si="0"/>
         <v>4014</v>
       </c>
       <c r="C6">
@@ -1063,16 +1097,16 @@
         <v>255</v>
       </c>
       <c r="E6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1275</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>25</v>
       </c>
       <c r="B7">
-        <f>B6+ E6+1</f>
+        <f t="shared" si="0"/>
         <v>5290</v>
       </c>
       <c r="C7">
@@ -1082,16 +1116,16 @@
         <v>255</v>
       </c>
       <c r="E7">
-        <f t="shared" ref="E7" si="1">C7*D7</f>
+        <f t="shared" ref="E7" si="2">C7*D7</f>
         <v>2040</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>26</v>
       </c>
       <c r="B8">
-        <f>B7+ E7+1</f>
+        <f t="shared" si="0"/>
         <v>7331</v>
       </c>
       <c r="C8">
@@ -1101,16 +1135,16 @@
         <v>255</v>
       </c>
       <c r="E8">
-        <f t="shared" ref="E8" si="2">C8*D8</f>
+        <f t="shared" ref="E8" si="3">C8*D8</f>
         <v>510</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>33</v>
       </c>
       <c r="B9">
-        <f>B8+ E8+1</f>
+        <f t="shared" si="0"/>
         <v>7842</v>
       </c>
       <c r="C9">
@@ -1120,11 +1154,11 @@
         <v>20</v>
       </c>
       <c r="E9">
-        <f t="shared" ref="E9" si="3">C9*D9</f>
+        <f t="shared" ref="E9" si="4">C9*D9</f>
         <v>200</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>2</v>
       </c>
@@ -1147,12 +1181,12 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -1169,7 +1203,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -1187,7 +1221,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>29</v>
       </c>
@@ -1206,7 +1240,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>32</v>
       </c>
@@ -1225,8 +1259,8 @@
         <v>256</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
         <v>30</v>
       </c>
       <c r="E10">
@@ -1234,7 +1268,7 @@
         <v>768</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>31</v>
       </c>

</xml_diff>

<commit_message>
Bug fixes for ViewTab
</commit_message>
<xml_diff>
--- a/doc/allocation.xlsx
+++ b/doc/allocation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\meka\CommanderX16Version\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F9B794A-F2EE-4145-AE22-F843105616DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8C6C265-48C3-451E-90CB-CDABD07BC853}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="34620" windowHeight="14020" activeTab="2" xr2:uid="{02454ED2-5616-494F-84FC-2DE3FC8B32E3}"/>
+    <workbookView minimized="1" xWindow="16000" yWindow="5110" windowWidth="3560" windowHeight="5440" activeTab="4" xr2:uid="{02454ED2-5616-494F-84FC-2DE3FC8B32E3}"/>
   </bookViews>
   <sheets>
     <sheet name="Dynamic" sheetId="2" r:id="rId1"/>
@@ -895,7 +895,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A86A6CAE-A2FB-4700-AF3B-F451BF94FBFE}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
@@ -1199,8 +1199,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF57E188-51E7-49EE-9F4F-07D9A5354CD1}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1271,14 +1271,14 @@
         <v>514</v>
       </c>
       <c r="C4">
-        <v>256</v>
+        <v>500</v>
       </c>
       <c r="D4">
         <v>1</v>
       </c>
       <c r="E4">
         <f t="shared" ref="E4" si="1">C4*D4</f>
-        <v>256</v>
+        <v>500</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
@@ -1287,7 +1287,7 @@
       </c>
       <c r="E10">
         <f>SUM(E2:E9)</f>
-        <v>768</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">

</xml_diff>